<commit_message>
uploading file with ScreenShots
updated
</commit_message>
<xml_diff>
--- a/Mile Killers/Team Step Count - Mile Killers.xlsx
+++ b/Mile Killers/Team Step Count - Mile Killers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lokesh Antii\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7D89B48-9111-4FEB-904E-5336D6263F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4A7521-5F0F-4565-9013-4131F7B53F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{285D0F21-9A7A-4F26-89F7-31D1B74F5187}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="ScreenShots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>#LetsGetHealthy - WALKATHON CHALLENGE</t>
   </si>
@@ -88,13 +89,19 @@
   </si>
   <si>
     <t>Mile Killers</t>
+  </si>
+  <si>
+    <t>First Week</t>
+  </si>
+  <si>
+    <t>Weekly Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +125,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -133,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -182,11 +197,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -208,6 +260,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,6 +291,474 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>83821</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>74295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>603571</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3650E771-1E22-4A37-BC22-F26D02003A7C}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="83821" y="312420"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>89535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>588330</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>65160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{998E083A-BC26-47D5-BB92-5A7A69559C7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3402330" y="327660"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>70486</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70485</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590236</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>46110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{046DD295-B9C5-40CE-9DF0-61A2C5F883AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6737986" y="308610"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>64770</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>74295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>584520</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A440CC60-B674-4AFD-AE36-F641D64F64AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10066020" y="312420"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>51435</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>74295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571185</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>49920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB0F0A8-A28A-4F38-A9EA-D923B8563F9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="51435" y="5627370"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>595950</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>25155</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C31B29F-507F-42ED-929A-92DA8E00C612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3409950" y="5602605"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>87630</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>607380</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C76334B-486E-40FB-A28A-E17569F46E7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6755130" y="6343650"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>74295</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>594045</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>34680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D4E1E72-12EF-485B-8A53-7AB49F9673C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10075545" y="5612130"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>80011</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>599761</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>63255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F11A0C7D-F223-4BA0-9564-BD71B26DEADC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13415011" y="5640705"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>586425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>51825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09376C77-539D-4A0A-AD1C-2F27BDACB507}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13401675" y="314325"/>
+          <a:ext cx="2520000" cy="4500000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936963F7-DD82-468F-BF30-E72F6B7A07DF}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,14 +1079,14 @@
     <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -559,7 +1095,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -568,7 +1104,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -577,7 +1113,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -586,14 +1122,23 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -603,8 +1148,26 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F7" s="16">
+        <v>44165</v>
+      </c>
+      <c r="G7" s="16">
+        <v>44166</v>
+      </c>
+      <c r="H7" s="16">
+        <v>44167</v>
+      </c>
+      <c r="I7" s="16">
+        <v>44168</v>
+      </c>
+      <c r="J7" s="16">
+        <v>44169</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -614,8 +1177,29 @@
       <c r="C8" s="3">
         <v>88881</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="17">
+        <v>18123</v>
+      </c>
+      <c r="G8" s="17">
+        <v>12420</v>
+      </c>
+      <c r="H8" s="17">
+        <v>16948</v>
+      </c>
+      <c r="I8" s="17">
+        <v>17809</v>
+      </c>
+      <c r="J8" s="17">
+        <v>23581</v>
+      </c>
+      <c r="K8" s="18">
+        <v>88881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -625,8 +1209,29 @@
       <c r="C9" s="3">
         <v>46102</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="17">
+        <v>2425</v>
+      </c>
+      <c r="G9" s="17">
+        <v>8131</v>
+      </c>
+      <c r="H9" s="17">
+        <v>11830</v>
+      </c>
+      <c r="I9" s="17">
+        <v>17479</v>
+      </c>
+      <c r="J9" s="17">
+        <v>6237</v>
+      </c>
+      <c r="K9" s="18">
+        <v>46102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -636,8 +1241,29 @@
       <c r="C10" s="3">
         <v>38480</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="17">
+        <v>7803</v>
+      </c>
+      <c r="G10" s="17">
+        <v>6649</v>
+      </c>
+      <c r="H10" s="17">
+        <v>7898</v>
+      </c>
+      <c r="I10" s="17">
+        <v>7351</v>
+      </c>
+      <c r="J10" s="17">
+        <v>8779</v>
+      </c>
+      <c r="K10" s="18">
+        <v>38480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -647,8 +1273,29 @@
       <c r="C11" s="3">
         <v>37896</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="17">
+        <v>5116</v>
+      </c>
+      <c r="G11" s="17">
+        <v>5138</v>
+      </c>
+      <c r="H11" s="17">
+        <v>4924</v>
+      </c>
+      <c r="I11" s="17">
+        <v>4785</v>
+      </c>
+      <c r="J11" s="17">
+        <v>17933</v>
+      </c>
+      <c r="K11" s="18">
+        <v>37896</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -658,8 +1305,29 @@
       <c r="C12" s="3">
         <v>32684</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="17">
+        <v>172</v>
+      </c>
+      <c r="G12" s="17">
+        <v>9370</v>
+      </c>
+      <c r="H12" s="17">
+        <v>8903</v>
+      </c>
+      <c r="I12" s="17">
+        <v>9080</v>
+      </c>
+      <c r="J12" s="17">
+        <v>5159</v>
+      </c>
+      <c r="K12" s="18">
+        <v>32684</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -669,8 +1337,29 @@
       <c r="C13" s="3">
         <v>24907</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="17">
+        <v>2882</v>
+      </c>
+      <c r="G13" s="17">
+        <v>81</v>
+      </c>
+      <c r="H13" s="17">
+        <v>1967</v>
+      </c>
+      <c r="I13" s="17">
+        <v>9144</v>
+      </c>
+      <c r="J13" s="17">
+        <v>10833</v>
+      </c>
+      <c r="K13" s="18">
+        <v>24907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -680,8 +1369,29 @@
       <c r="C14" s="3">
         <v>17356</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="17">
+        <v>579</v>
+      </c>
+      <c r="G14" s="17">
+        <v>4080</v>
+      </c>
+      <c r="H14" s="17">
+        <v>4192</v>
+      </c>
+      <c r="I14" s="17">
+        <v>7201</v>
+      </c>
+      <c r="J14" s="17">
+        <v>1304</v>
+      </c>
+      <c r="K14" s="18">
+        <v>17356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -691,8 +1401,29 @@
       <c r="C15" s="3">
         <v>16326</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
+        <v>661</v>
+      </c>
+      <c r="H15" s="17">
+        <v>2085</v>
+      </c>
+      <c r="I15" s="17">
+        <v>4314</v>
+      </c>
+      <c r="J15" s="17">
+        <v>9266</v>
+      </c>
+      <c r="K15" s="18">
+        <v>16326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -702,8 +1433,29 @@
       <c r="C16" s="3">
         <v>14207</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="17">
+        <v>4863</v>
+      </c>
+      <c r="G16" s="17">
+        <v>3576</v>
+      </c>
+      <c r="H16" s="17">
+        <v>140</v>
+      </c>
+      <c r="I16" s="17">
+        <v>5467</v>
+      </c>
+      <c r="J16" s="17">
+        <v>161</v>
+      </c>
+      <c r="K16" s="18">
+        <v>14207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -713,8 +1465,29 @@
       <c r="C17" s="3">
         <v>13855</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="17">
+        <v>370</v>
+      </c>
+      <c r="G17" s="17">
+        <v>3179</v>
+      </c>
+      <c r="H17" s="17">
+        <v>838</v>
+      </c>
+      <c r="I17" s="17">
+        <v>6426</v>
+      </c>
+      <c r="J17" s="17">
+        <v>3042</v>
+      </c>
+      <c r="K17" s="18">
+        <v>13855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
@@ -728,7 +1501,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E8:K17">
     <sortCondition descending="1" ref="K8:K17"/>
   </sortState>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="E6:K6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A18:B18"/>
@@ -740,4 +1514,101 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017FE54D-27A7-4F43-AF04-99CEAB9DDDC4}">
+  <dimension ref="A1:X30"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="24" width="9.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="F1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="K1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="P1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="14"/>
+      <c r="U1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="14"/>
+    </row>
+    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:24" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="F30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
+      <c r="K30" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
+      <c r="P30" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="14"/>
+      <c r="U30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="P30:S30"/>
+    <mergeCell ref="U30:X30"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="K30:N30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>